<commit_message>
change qr codes and add savefig
</commit_message>
<xml_diff>
--- a/QR Codes.xlsx
+++ b/QR Codes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\python_account\Documents\GitHub\Christmas-Tree-FMIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spenc\Christmas-Tree-FMIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6279A2E-E8A3-46AD-9FE8-B9EF6B5C05B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F17FED-9215-4E98-AC40-30AA20B69769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{811682B6-46C0-4652-BC25-434E177B5E4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{811682B6-46C0-4652-BC25-434E177B5E4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,27 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Task Description</t>
+    <t>Open Space</t>
   </si>
   <si>
-    <t>new tree</t>
+    <t>Dead Tree</t>
   </si>
   <si>
-    <t>stump culture</t>
+    <t>Pest Issue</t>
   </si>
   <si>
-    <t>insects</t>
-  </si>
-  <si>
-    <t>irrigation</t>
-  </si>
-  <si>
-    <t>stuff</t>
-  </si>
-  <si>
-    <t>Task Completion Barcode</t>
+    <t>2023 Sapling</t>
   </si>
 </sst>
 </file>
@@ -104,23 +95,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>120651</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>187325</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>274152</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>657225</xdr:rowOff>
+      <xdr:rowOff>2714625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2">
+        <xdr:cNvPr id="12" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EF4A132-8E0E-7F55-1994-FEC507E95B81}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97B36A73-9C72-3C0A-6244-3ADEAD7850C3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -136,8 +127,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1057275" y="85725"/>
-          <a:ext cx="952500" cy="952500"/>
+          <a:off x="120651" y="568325"/>
+          <a:ext cx="2518876" cy="2527300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -148,23 +139,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3175</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>2565400</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>682625</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2746375</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 3">
+        <xdr:cNvPr id="15" name="Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74746476-FE5B-3D6D-CE1A-3063AA09B959}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8899DA31-81B7-E5CF-E4BB-1638FDC27E07}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -180,8 +171,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1035050" y="2946400"/>
-          <a:ext cx="949325" cy="952500"/>
+          <a:off x="3048000" y="558800"/>
+          <a:ext cx="2568575" cy="2568575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -192,23 +183,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>390525</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>79376</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>533401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>355601</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>1343025</xdr:rowOff>
+      <xdr:rowOff>825501</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 4">
+        <xdr:cNvPr id="16" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7952B728-D1B0-FA31-518B-978066C9A12A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F84E236-B588-E1BA-E7BE-C4401BEFBD4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -224,8 +215,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1079500" y="4359275"/>
-          <a:ext cx="949325" cy="952500"/>
+          <a:off x="79376" y="4327526"/>
+          <a:ext cx="2641600" cy="2641600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -236,23 +227,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>2263775</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>650876</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>558801</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>136525</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>536576</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>889001</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 5">
+        <xdr:cNvPr id="17" name="Picture 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C084D4DB-BAE5-8226-556E-E8A92AB2FE0E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC633750-B586-F888-9A8F-5A4C9C99D772}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -268,272 +259,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1060450" y="11550650"/>
-          <a:ext cx="949325" cy="952500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>996950</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>4883150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>184150</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B31D373B-3CE7-975B-3655-4B302541D5AA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="996950" y="17440275"/>
-          <a:ext cx="949325" cy="946150"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>765175</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{660B12DA-B4E3-5AFB-95CA-632BB980F85E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3990975" y="190500"/>
-          <a:ext cx="952500" cy="952500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>2600325</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>155575</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCCB6888-8B81-9B1E-46F2-7EF4C37DD907}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3962400" y="2981325"/>
-          <a:ext cx="946150" cy="952500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>428625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1381125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51A4CD03-32C9-7E96-946A-2236AA1B56F2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3889375" y="4397375"/>
-          <a:ext cx="946150" cy="952500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>34925</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>2222500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>377825</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{458356B2-8AA9-0620-B92A-4518EC411025}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3987800" y="11509375"/>
-          <a:ext cx="946150" cy="952500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>4892675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DA15B4A-E97C-CDB2-C0D0-16220B723CD1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3971925" y="17449800"/>
-          <a:ext cx="946150" cy="949325"/>
+          <a:off x="3016251" y="4352926"/>
+          <a:ext cx="2679700" cy="2679700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -842,7 +569,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -862,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78C5086-D781-4CC7-AAFE-82757C90EA0B}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A2:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,85 +602,30 @@
     <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
+      <c r="D2" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="3" spans="1:5" ht="251.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
       </c>
-      <c r="D2" t="str">
-        <f xml:space="preserve"> IF(A2&lt;&gt;"",_xlfn.CONCAT("COMP ",A2),"")</f>
-        <v>COMP new tree</v>
+      <c r="E4" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="251.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:4" ht="252" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" t="str">
-        <f t="shared" ref="D4:D12" si="0" xml:space="preserve"> IF(A4&lt;&gt;"",_xlfn.CONCAT("COMP ",A4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>COMP stump culture</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="128.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" ht="403.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>COMP insects</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="242.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>COMP irrigation</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>COMP stuff</v>
-      </c>
-    </row>
+    <row r="5" spans="1:5" ht="169.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:5" ht="128.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:5" ht="403.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:5" ht="242.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="71.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>